<commit_message>
report but no table of contents
</commit_message>
<xml_diff>
--- a/reports/report-1/Project charter but excel.xlsx
+++ b/reports/report-1/Project charter but excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CurSold-PC\Desktop\Github project\on-campus-delivery-robot\reports\report-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8D8495-ACCA-4552-AFF8-BD905BE9B2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9C5E49-B80F-4BF2-976A-D4F1EDB619B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>1.General Project Information</t>
   </si>
@@ -112,13 +112,100 @@
   </si>
   <si>
     <t>Objectives</t>
+  </si>
+  <si>
+    <t>Project Purpose</t>
+  </si>
+  <si>
+    <t>Musts</t>
+  </si>
+  <si>
+    <t>Wants</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Project Deliverables</t>
+  </si>
+  <si>
+    <t>Project Milestones</t>
+  </si>
+  <si>
+    <t>Risks &amp; Remedies</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Remedy</t>
+  </si>
+  <si>
+    <t>Roles  &amp; Responsibilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role </t>
+  </si>
+  <si>
+    <t>Technical Role</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>Dr.Muhammed Bilal</t>
+  </si>
+  <si>
+    <t>Help the team reach the final solution while meeting the customers requirements.</t>
+  </si>
+  <si>
+    <t>Requests a solution with given specifications and requirements.</t>
+  </si>
+  <si>
+    <t>Idea challenger, Recorder</t>
+  </si>
+  <si>
+    <t>Organizer, Gatekeeper</t>
+  </si>
+  <si>
+    <t>Team leader/ Project manger</t>
+  </si>
+  <si>
+    <t>navigating algorithms</t>
+  </si>
+  <si>
+    <t>Obstacle avoidance algorithms</t>
+  </si>
+  <si>
+    <t>hardware &amp; code deployment</t>
+  </si>
+  <si>
+    <t>Plays the role of the devil’s advocate, types the meeting minutes</t>
+  </si>
+  <si>
+    <t>Organizes team meetings time and place and the meeting outcomes, ensures that all goals are achieved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Planning and organizing the completion of tasks within the project</t>
+  </si>
+  <si>
+    <t>Sign Off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,8 +245,34 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +290,14 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -214,22 +333,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -243,15 +414,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,9 +421,92 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
     <cellStyle name="Accent5" xfId="2" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -541,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E12:O18"/>
+  <dimension ref="E12:AH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:O16"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AE12" sqref="AE12:AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,141 +802,410 @@
     <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="71.85546875" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="22.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
+    <row r="12" spans="5:34" x14ac:dyDescent="0.25">
+      <c r="E12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="K12" s="4" t="s">
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="K12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="N12" s="1" t="s">
+      <c r="L12" s="19"/>
+      <c r="N12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-      <c r="F13" s="10" t="s">
+      <c r="O12" s="18"/>
+      <c r="Q12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="18"/>
+      <c r="S12" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="T12" s="27"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AB12" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC12" s="35"/>
+      <c r="AE12" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
+      <c r="AH12" s="32"/>
+    </row>
+    <row r="13" spans="5:34" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+      <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="L13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="N13" s="17" t="s">
+      <c r="N13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E14" s="11" t="s">
+      <c r="O13" s="2"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="2"/>
+      <c r="V13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W13" s="15"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AB13" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC13" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE13" s="42"/>
+      <c r="AF13" s="42"/>
+      <c r="AG13" s="42"/>
+      <c r="AH13" s="42"/>
+    </row>
+    <row r="14" spans="5:34" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="11" t="s">
+      <c r="O14" s="2"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="2"/>
+      <c r="V14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W14" s="30"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="36"/>
+      <c r="AE14" s="42"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="36"/>
+      <c r="AH14" s="36"/>
+    </row>
+    <row r="15" spans="5:34" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="K15" s="5" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="K15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="17" t="s">
+      <c r="N15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="14" t="s">
+      <c r="O15" s="2"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="2"/>
+      <c r="V15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="W15" s="30"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AB15" s="36"/>
+      <c r="AC15" s="36"/>
+      <c r="AE15" s="42"/>
+      <c r="AF15" s="36"/>
+      <c r="AG15" s="36"/>
+      <c r="AH15" s="36"/>
+    </row>
+    <row r="16" spans="5:34" x14ac:dyDescent="0.25">
+      <c r="E16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="22"/>
+      <c r="H16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="17" t="s">
+      <c r="N16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="14"/>
-      <c r="F17" s="15" t="s">
+      <c r="O16" s="2"/>
+      <c r="V16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="W16" s="30"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AB16" s="36"/>
+      <c r="AC16" s="36"/>
+      <c r="AE16" s="42"/>
+      <c r="AF16" s="36"/>
+      <c r="AG16" s="36"/>
+      <c r="AH16" s="36"/>
+    </row>
+    <row r="17" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E17" s="20"/>
+      <c r="F17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="22"/>
+      <c r="H17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="14"/>
-      <c r="F18" s="15" t="s">
+      <c r="V17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W17" s="31"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AB17" s="36"/>
+      <c r="AC17" s="36"/>
+    </row>
+    <row r="18" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="E18" s="20"/>
+      <c r="F18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="22"/>
+      <c r="H18" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="36"/>
+    </row>
+    <row r="19" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+    </row>
+    <row r="20" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+    </row>
+    <row r="21" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N21" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+    </row>
+    <row r="22" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q22" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+    </row>
+    <row r="23" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N23" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="P23" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q23" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+    </row>
+    <row r="24" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O26" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P26" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N27" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="P27" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q27" s="41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N28" s="38"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+    </row>
+    <row r="29" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N29" s="12"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+    </row>
+    <row r="30" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N30" s="12"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+    </row>
+    <row r="31" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N31" s="12"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+    </row>
+    <row r="32" spans="5:29" x14ac:dyDescent="0.25">
+      <c r="N32" s="12"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+    </row>
+    <row r="33" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N33" s="12"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="16">
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="AE12:AH12"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="N21:Q21"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="Q12:R12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="E12:H12"/>
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="N12:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>